<commit_message>
Coupon Code Field Added in Sales Report
</commit_message>
<xml_diff>
--- a/Public/sales-report/sales_report.xlsx
+++ b/Public/sales-report/sales_report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="37">
   <si>
     <t>Order ID</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Discount</t>
   </si>
   <si>
+    <t>Coupon Code</t>
+  </si>
+  <si>
     <t>Total Amount</t>
   </si>
   <si>
@@ -95,18 +98,6 @@
   </si>
   <si>
     <t>order_MtTYIlWvk0hnp7</t>
-  </si>
-  <si>
-    <t>order_Mu1fpsNNLn2cNV</t>
-  </si>
-  <si>
-    <t>faiz</t>
-  </si>
-  <si>
-    <t>groove@gmail.com</t>
-  </si>
-  <si>
-    <t>{"addressType":"Home Address","name":"faiz","city":"fort Kochi","landMark":"Near Govt Higher Secondary School","state":"Kerala","pincode":6754266,"phone":7902427009,"altPhone":9088753267}</t>
   </si>
   <si>
     <t>ref4337fgh37747</t>
@@ -517,13 +508,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:N12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="13" width="30" style="1" customWidth="1"/>
+    <col min="1" max="14" width="30" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -563,22 +554,25 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="1">
         <v>0</v>
@@ -586,14 +580,12 @@
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1">
         <v>19499</v>
       </c>
-      <c r="I2" s="3">
+      <c r="J2" s="3">
         <v>45224.16333635416</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>19</v>
@@ -601,25 +593,28 @@
       <c r="L2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="3">
+      <c r="M2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="3">
         <v>45224.16333635416</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1">
         <v>0</v>
@@ -627,163 +622,167 @@
       <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="1"/>
+      <c r="I3" s="1">
         <v>19499</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="3">
         <v>45224.62502172454</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="3">
+        <v>45224.62502172454</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="3">
-        <v>45224.62502172454</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F4" s="1">
         <v>0</v>
       </c>
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4" s="1"/>
+      <c r="I4" s="1">
         <v>15998</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>45226.53042122685</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" s="3">
+        <v>45226.53042122685</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="3">
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1">
+        <v>15998</v>
+      </c>
+      <c r="J5" s="3">
         <v>45226.53042122685</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1">
-        <v>15998</v>
-      </c>
-      <c r="I5" s="3">
-        <v>45226.53042122685</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="K5" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="3">
+        <v>45226.53042122685</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M5" s="3">
-        <v>45226.53042122685</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="F6" s="1">
         <v>0</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1">
         <v>7999</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <v>45197.13755987269</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M6" s="3">
+        <v>20</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" s="3">
         <v>45197.13755987269</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -791,268 +790,233 @@
       <c r="G7" s="1">
         <v>0</v>
       </c>
-      <c r="H7" s="1">
-        <v>19499</v>
-      </c>
-      <c r="I7" s="3">
-        <v>45228.52832762731</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>18</v>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1">
+        <v>83993</v>
+      </c>
+      <c r="J7" s="3">
+        <v>45229.58961476852</v>
       </c>
       <c r="K7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="L7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="3">
+        <v>45229.58961476852</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1">
+        <v>83993</v>
+      </c>
+      <c r="J8" s="3">
+        <v>45229.58961476852</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="3">
+        <v>45229.58961476852</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1">
+        <v>83993</v>
+      </c>
+      <c r="J9" s="3">
+        <v>45229.58961476852</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N9" s="3">
+        <v>45229.58961476852</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M7" s="3">
-        <v>45228.52832762731</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1">
+        <v>89497</v>
+      </c>
+      <c r="J10" s="3">
+        <v>45230.21572832176</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="M10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N10" s="3">
+        <v>45230.21572832176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1">
+        <v>89497</v>
+      </c>
+      <c r="J11" s="3">
+        <v>45230.21572832176</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11" s="3">
+        <v>45230.21572832176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>83993</v>
-      </c>
-      <c r="I8" s="3">
-        <v>45229.58961476852</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M8" s="3">
-        <v>45229.58961476852</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1">
+        <v>89497</v>
+      </c>
+      <c r="J12" s="3">
+        <v>45230.21572832176</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>83993</v>
-      </c>
-      <c r="I9" s="3">
-        <v>45229.58961476852</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M9" s="3">
-        <v>45229.58961476852</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>83993</v>
-      </c>
-      <c r="I10" s="3">
-        <v>45229.58961476852</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M10" s="3">
-        <v>45229.58961476852</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>89497</v>
-      </c>
-      <c r="I11" s="3">
-        <v>45230.21572832176</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M11" s="3">
-        <v>45230.21572832176</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1">
-        <v>89497</v>
-      </c>
-      <c r="I12" s="3">
-        <v>45230.21572832176</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M12" s="3">
-        <v>45230.21572832176</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1">
-        <v>89497</v>
-      </c>
-      <c r="I13" s="3">
-        <v>45230.21572832176</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M13" s="3">
+      <c r="M12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N12" s="3">
         <v>45230.21572832176</v>
       </c>
     </row>

</xml_diff>